<commit_message>
old pistols as samples
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,9 +474,12 @@
           <t>طالب</t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>C:\Users\Abdallah Reda\Downloads\CVC-19-Documnet-Wallet-\BackEnd\visionapp\Natinal_ID\src\project\results\df\1_result.jpg</t>
+          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\1_result.jpg</t>
         </is>
       </c>
     </row>
@@ -501,9 +504,12 @@
           <t>طالب</t>
         </is>
       </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>C:\Users\Abdallah Reda\Downloads\CVC-19-Documnet-Wallet-\BackEnd\visionapp\Natinal_ID\src\project\results\df\2_result.jpg</t>
+          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\2_result.jpg</t>
         </is>
       </c>
     </row>
@@ -528,9 +534,12 @@
           <t>طالب</t>
         </is>
       </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>C:\Users\Abdallah Reda\Downloads\CVC-19-Documnet-Wallet-\BackEnd\visionapp\Natinal_ID\src\project\results\df\3_result.jpg</t>
+          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\3_result.jpg</t>
         </is>
       </c>
     </row>
@@ -555,9 +564,12 @@
           <t>طالب</t>
         </is>
       </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>C:\Users\Abdallah Reda\Downloads\CVC-19-Documnet-Wallet-\BackEnd\visionapp\Natinal_ID\src\project\results\df\4_result.jpg</t>
+          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\4_result.jpg</t>
         </is>
       </c>
     </row>
@@ -582,9 +594,72 @@
           <t>طالب</t>
         </is>
       </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>C:\Users\Abdallah Reda\Downloads\CVC-19-Documnet-Wallet-\BackEnd\visionapp\Natinal_ID\src\project\results\df\5_result.jpg</t>
+          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\5_result.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>490</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>نورالدين عبدالحميد</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>طالب</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\6_result.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>505</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>محمد صبحى احمد</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>طالب</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\7_result.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding working conf.ini file
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,66 +603,6 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>490</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>نورالدين عبدالحميد</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>طالب</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\6_result.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>505</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>محمد صبحى احمد</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>طالب</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\7_result.jpg</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
featGUI: change targets and bullets if gun changed
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,156 +453,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>564</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>مينا جوزيف متري</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>طالب</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\1_result.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ايهاب محمد شعبان</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>طالب</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\2_result.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>435</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>محمد سعيد احمد</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>طالب</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\3_result.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>449</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>احمد عطوه السيد</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>طالب</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\4_result.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>احمد هشام ابو خليفه</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>طالب</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>C:\Users\GreaTiger\Desktop\project\results\السرية الثامنة\5_result.jpg</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>